<commit_message>
update logo for btue
</commit_message>
<xml_diff>
--- a/src/main/java/utility/logo.xlsx
+++ b/src/main/java/utility/logo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\project3ds\src\main\java\utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D262F215-0468-4C9D-900C-4FD2C97391A5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10F5EAB-007C-404D-893A-8D95757B599C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8415" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20385" yWindow="-10920" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="psname" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="454">
   <si>
     <t>efectycolombia</t>
   </si>
@@ -1376,6 +1376,24 @@
   </si>
   <si>
     <t>BankTransferThailand</t>
+  </si>
+  <si>
+    <t>bteu</t>
+  </si>
+  <si>
+    <t>FasterPay / Bank Transfer</t>
+  </si>
+  <si>
+    <t>FasterPay   Bank transfer</t>
+  </si>
+  <si>
+    <t>Uberweisung</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>tab_bteu</t>
   </si>
 </sst>
 </file>
@@ -1600,7 +1618,24 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2032,8 +2067,8 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K49" sqref="K49"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3215,7 +3250,7 @@
     </row>
     <row r="40" spans="1:9" ht="16.5" thickBot="1">
       <c r="A40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40">
         <f>VLOOKUP(C40,shortcode!$B$1:$C$200,2,FALSE)</f>
@@ -3482,15 +3517,52 @@
         <v>431</v>
       </c>
     </row>
-    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="49" spans="1:9" ht="15.75">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>288</v>
+      </c>
+      <c r="C49" t="s">
+        <v>448</v>
+      </c>
+      <c r="D49" t="s">
+        <v>449</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>450</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>451</v>
+      </c>
+      <c r="G49">
+        <v>76</v>
+      </c>
+      <c r="H49" s="18" t="s">
+        <v>452</v>
+      </c>
+      <c r="I49" s="18" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="14.25" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="G3:G48 H48:I48">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>COUNTIF($Q$3:$AD$3,G3)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G48 H48:I48">
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G49:I49">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>COUNTIF($Q$3:$AD$3,G49)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G49:I49">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4180,59 +4252,59 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:C74">
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>COUNTIF($P$3:$AC$3,B2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75:C75">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="15" priority="11">
       <formula>COUNTIF($P$3:$AC$3,B75)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76:C76">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>COUNTIF($P$3:$AC$3,B76)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77:C82">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>COUNTIF($P$3:$AC$3,B77)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77:C82">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77:B82">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:C83">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>COUNTIF($P$3:$AC$3,B83)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C74">
-    <cfRule type="duplicateValues" dxfId="1" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B74">
-    <cfRule type="duplicateValues" dxfId="0" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="21"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update logo dark and logo name
</commit_message>
<xml_diff>
--- a/src/main/java/utility/logo.xlsx
+++ b/src/main/java/utility/logo.xlsx
@@ -8,15 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\project3ds\src\main\java\utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482D6CE1-D6CA-4FF5-9ECB-2AA34C35B0AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A62BEBB-C2C1-41EB-822E-E7909B37B327}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8415" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20385" yWindow="-10920" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="psname" sheetId="1" r:id="rId1"/>
     <sheet name="country" sheetId="2" r:id="rId2"/>
     <sheet name="shortcode" sheetId="3" r:id="rId3"/>
+    <sheet name="logoName" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">psname!$A$1:$J$49</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="514">
   <si>
     <t>efectycolombia</t>
   </si>
@@ -1394,13 +1398,193 @@
   </si>
   <si>
     <t>tab_bteu</t>
+  </si>
+  <si>
+    <t>PS name</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>Logo name</t>
+  </si>
+  <si>
+    <t>Zong</t>
+  </si>
+  <si>
+    <t>zong</t>
+  </si>
+  <si>
+    <t>sms</t>
+  </si>
+  <si>
+    <t>Paymo</t>
+  </si>
+  <si>
+    <t>paymo</t>
+  </si>
+  <si>
+    <t>Credit card</t>
+  </si>
+  <si>
+    <t>socialgold</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>Smscoin</t>
+  </si>
+  <si>
+    <t>smscoin</t>
+  </si>
+  <si>
+    <t>Allopass</t>
+  </si>
+  <si>
+    <t>allopass</t>
+  </si>
+  <si>
+    <t>MikroOdeme</t>
+  </si>
+  <si>
+    <t>mikroodeme</t>
+  </si>
+  <si>
+    <t>Bank Transfer</t>
+  </si>
+  <si>
+    <t>webbilling</t>
+  </si>
+  <si>
+    <t>banktransfer</t>
+  </si>
+  <si>
+    <t>Directpay</t>
+  </si>
+  <si>
+    <t>directpay</t>
+  </si>
+  <si>
+    <t>Fortumo</t>
+  </si>
+  <si>
+    <t>fortumo</t>
+  </si>
+  <si>
+    <t>TrustPay</t>
+  </si>
+  <si>
+    <t>trustpay</t>
+  </si>
+  <si>
+    <t>Credit Cards Dotpay</t>
+  </si>
+  <si>
+    <t>dotpaycc</t>
+  </si>
+  <si>
+    <t>Landline Payments</t>
+  </si>
+  <si>
+    <t>landline</t>
+  </si>
+  <si>
+    <t>allopasscc</t>
+  </si>
+  <si>
+    <t>mobiamo</t>
+  </si>
+  <si>
+    <t>cceuro</t>
+  </si>
+  <si>
+    <t>Credit Cards</t>
+  </si>
+  <si>
+    <t>mercadopagocc</t>
+  </si>
+  <si>
+    <t>mercadopagohiper</t>
+  </si>
+  <si>
+    <t>hiper</t>
+  </si>
+  <si>
+    <t>Elo Card</t>
+  </si>
+  <si>
+    <t>mercadopagoelo</t>
+  </si>
+  <si>
+    <t>elo</t>
+  </si>
+  <si>
+    <t>Teleingreso</t>
+  </si>
+  <si>
+    <t>teleingreso</t>
+  </si>
+  <si>
+    <t>cc3</t>
+  </si>
+  <si>
+    <t>Webmoney Japan</t>
+  </si>
+  <si>
+    <t>webmoneyjapan</t>
+  </si>
+  <si>
+    <t>webmoneyjp</t>
+  </si>
+  <si>
+    <t>cceu</t>
+  </si>
+  <si>
+    <t>cc4</t>
+  </si>
+  <si>
+    <t>Transferência bancária</t>
+  </si>
+  <si>
+    <t>btbrazil</t>
+  </si>
+  <si>
+    <t>Belfius</t>
+  </si>
+  <si>
+    <t>ccbrazil_flag</t>
+  </si>
+  <si>
+    <t>Credit Cards Korea</t>
+  </si>
+  <si>
+    <t>allthegate_flag</t>
+  </si>
+  <si>
+    <t>Bank transfer Finland</t>
+  </si>
+  <si>
+    <t>Mybank</t>
+  </si>
+  <si>
+    <t>Boleto Bancário</t>
+  </si>
+  <si>
+    <t>Multibanco</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>logo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1465,6 +1649,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF172B4D"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1480,7 +1669,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1564,12 +1753,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1613,12 +1822,23 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1744,6 +1964,214 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2064,11 +2492,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2077,9 +2505,11 @@
     <col min="4" max="4" width="37.7109375" customWidth="1"/>
     <col min="5" max="5" width="50.5703125" customWidth="1"/>
     <col min="6" max="6" width="42" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32.25" thickBot="1">
+    <row r="1" spans="1:10" ht="32.25" thickBot="1">
       <c r="A1" t="s">
         <v>435</v>
       </c>
@@ -2107,8 +2537,11 @@
       <c r="I1" s="7" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J1" s="7" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" thickBot="1">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2137,8 +2570,12 @@
       <c r="I2" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J2" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C2,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C2,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" thickBot="1">
       <c r="A3">
         <v>0</v>
       </c>
@@ -2167,8 +2604,12 @@
       <c r="I3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J3" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C3,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C3,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" thickBot="1">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2197,8 +2638,12 @@
       <c r="I4" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J4" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C4,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C4,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v>boleto</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" thickBot="1">
       <c r="A5">
         <v>0</v>
       </c>
@@ -2227,8 +2672,12 @@
       <c r="I5" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J5" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C5,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C5,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" thickBot="1">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2257,8 +2706,12 @@
       <c r="I6" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J6" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C6,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C6,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" thickBot="1">
       <c r="A7">
         <v>0</v>
       </c>
@@ -2287,8 +2740,12 @@
       <c r="I7" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J7" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C7,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C7,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v>ccbrazil_flag</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" thickBot="1">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2317,8 +2774,12 @@
       <c r="I8" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J8" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C8,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C8,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v>hipercard</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" thickBot="1">
       <c r="A9">
         <v>0</v>
       </c>
@@ -2347,8 +2808,12 @@
       <c r="I9" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J9" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C9,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C9,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" thickBot="1">
       <c r="A10">
         <v>0</v>
       </c>
@@ -2377,8 +2842,12 @@
       <c r="I10" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J10" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C10,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C10,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" thickBot="1">
       <c r="A11">
         <v>0</v>
       </c>
@@ -2407,8 +2876,12 @@
       <c r="I11" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J11" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C11,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C11,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16.5" thickBot="1">
       <c r="A12">
         <v>0</v>
       </c>
@@ -2437,8 +2910,12 @@
       <c r="I12" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J12" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C12,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C12,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" thickBot="1">
       <c r="A13">
         <v>0</v>
       </c>
@@ -2467,8 +2944,12 @@
       <c r="I13" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J13" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C13,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C13,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" thickBot="1">
       <c r="A14">
         <v>0</v>
       </c>
@@ -2497,8 +2978,12 @@
       <c r="I14" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J14" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C14,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C14,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16.5" thickBot="1">
       <c r="A15">
         <v>0</v>
       </c>
@@ -2527,8 +3012,12 @@
       <c r="I15" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J15" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C15,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C15,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" thickBot="1">
       <c r="A16">
         <v>0</v>
       </c>
@@ -2557,8 +3046,12 @@
       <c r="I16" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J16" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C16,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C16,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16.5" thickBot="1">
       <c r="A17">
         <v>0</v>
       </c>
@@ -2587,8 +3080,12 @@
       <c r="I17" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J17" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C17,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C17,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="16.5" thickBot="1">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2617,8 +3114,12 @@
       <c r="I18" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J18" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C18,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C18,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16.5" thickBot="1">
       <c r="A19">
         <v>0</v>
       </c>
@@ -2647,8 +3148,12 @@
       <c r="I19" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J19" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C19,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C19,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="16.5" thickBot="1">
       <c r="A20">
         <v>0</v>
       </c>
@@ -2677,8 +3182,12 @@
       <c r="I20" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J20" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C20,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C20,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="16.5" thickBot="1">
       <c r="A21">
         <v>0</v>
       </c>
@@ -2707,8 +3216,12 @@
       <c r="I21" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J21" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C21,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C21,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="16.5" thickBot="1">
       <c r="A22">
         <v>0</v>
       </c>
@@ -2737,8 +3250,12 @@
       <c r="I22" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J22" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C22,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C22,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="16.5" thickBot="1">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2767,8 +3284,12 @@
       <c r="I23" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J23" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C23,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C23,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v>allthegate_flag</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="16.5" thickBot="1">
       <c r="A24">
         <v>0</v>
       </c>
@@ -2797,8 +3318,12 @@
       <c r="I24" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J24" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C24,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C24,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="16.5" thickBot="1">
       <c r="A25">
         <v>0</v>
       </c>
@@ -2827,8 +3352,12 @@
       <c r="I25" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J25" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C25,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C25,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v>idealpayments</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="16.5" thickBot="1">
       <c r="A26">
         <v>0</v>
       </c>
@@ -2857,8 +3386,12 @@
       <c r="I26" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J26" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C26,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C26,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="16.5" thickBot="1">
       <c r="A27">
         <v>0</v>
       </c>
@@ -2887,8 +3420,12 @@
       <c r="I27" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J27" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C27,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C27,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="16.5" thickBot="1">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2917,8 +3454,12 @@
       <c r="I28" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J28" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C28,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C28,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="16.5" thickBot="1">
       <c r="A29">
         <v>0</v>
       </c>
@@ -2947,8 +3488,12 @@
       <c r="I29" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J29" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C29,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C29,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="16.5" thickBot="1">
       <c r="A30">
         <v>0</v>
       </c>
@@ -2977,8 +3522,12 @@
       <c r="I30" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J30" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C30,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C30,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v>boleto</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="16.5" thickBot="1">
       <c r="A31">
         <v>0</v>
       </c>
@@ -3007,8 +3556,12 @@
       <c r="I31" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J31" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C31,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C31,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v>ideal</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="16.5" thickBot="1">
       <c r="A32">
         <v>0</v>
       </c>
@@ -3037,8 +3590,12 @@
       <c r="I32" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J32" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C32,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C32,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="16.5" thickBot="1">
       <c r="A33">
         <v>0</v>
       </c>
@@ -3067,8 +3624,12 @@
       <c r="I33" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J33" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C33,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C33,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="16.5" thickBot="1">
       <c r="A34">
         <v>0</v>
       </c>
@@ -3097,8 +3658,12 @@
       <c r="I34" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J34" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C34,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C34,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="16.5" thickBot="1">
       <c r="A35">
         <v>0</v>
       </c>
@@ -3127,8 +3692,12 @@
       <c r="I35" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J35" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C35,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C35,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="16.5" thickBot="1">
       <c r="A36">
         <v>0</v>
       </c>
@@ -3157,8 +3726,12 @@
       <c r="I36" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J36" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C36,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C36,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="16.5" thickBot="1">
       <c r="A37">
         <v>0</v>
       </c>
@@ -3187,8 +3760,12 @@
       <c r="I37" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J37" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C37,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C37,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="16.5" thickBot="1">
       <c r="A38">
         <v>0</v>
       </c>
@@ -3217,8 +3794,12 @@
       <c r="I38" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J38" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C38,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C38,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="16.5" thickBot="1">
       <c r="A39">
         <v>0</v>
       </c>
@@ -3247,8 +3828,12 @@
       <c r="I39" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J39" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C39,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C39,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="16.5" thickBot="1">
       <c r="A40">
         <v>0</v>
       </c>
@@ -3277,10 +3862,14 @@
       <c r="I40" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J40" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C40,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C40,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="16.5" thickBot="1">
       <c r="A41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B41">
         <f>VLOOKUP(C41,shortcode!$B$1:$C$200,2,FALSE)</f>
@@ -3307,10 +3896,14 @@
       <c r="I41" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J41" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C41,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C41,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="16.5" thickBot="1">
       <c r="A42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B42">
         <f>VLOOKUP(C42,shortcode!$B$1:$C$200,2,FALSE)</f>
@@ -3337,8 +3930,12 @@
       <c r="I42" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J42" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C42,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C42,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="16.5" thickBot="1">
       <c r="A43">
         <v>0</v>
       </c>
@@ -3367,8 +3964,12 @@
       <c r="I43" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J43" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C43,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C43,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v>epspayments</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="16.5" thickBot="1">
       <c r="A44">
         <v>0</v>
       </c>
@@ -3397,8 +3998,12 @@
       <c r="I44" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J44" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C44,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C44,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="16.5" thickBot="1">
       <c r="A45">
         <v>0</v>
       </c>
@@ -3427,8 +4032,12 @@
       <c r="I45" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J45" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C45,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C45,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v>multibanco</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="16.5" thickBot="1">
       <c r="A46">
         <v>0</v>
       </c>
@@ -3457,8 +4066,12 @@
       <c r="I46" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="16.5" thickBot="1">
+      <c r="J46" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C46,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C46,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v>mint</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="16.5" thickBot="1">
       <c r="A47">
         <v>0</v>
       </c>
@@ -3487,8 +4100,12 @@
       <c r="I47" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75">
+      <c r="J47" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C47,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C47,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="16.5" thickBot="1">
       <c r="A48">
         <v>0</v>
       </c>
@@ -3516,53 +4133,66 @@
       <c r="I48" s="18" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75">
+      <c r="J48" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C48,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C48,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="21" customFormat="1" ht="16.5" thickBot="1">
       <c r="A49">
         <v>0</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="21">
         <v>288</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="21" t="s">
         <v>448</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="21" t="s">
         <v>449</v>
       </c>
-      <c r="E49" s="17" t="s">
+      <c r="E49" s="22" t="s">
         <v>450</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="F49" s="22" t="s">
         <v>451</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="21">
         <v>76</v>
       </c>
-      <c r="H49" s="18" t="s">
+      <c r="H49" s="23" t="s">
         <v>452</v>
       </c>
-      <c r="I49" s="18" t="s">
+      <c r="I49" s="23" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="14.25" customHeight="1"/>
+      <c r="J49" s="3" t="str">
+        <f>IF(ISNA(VLOOKUP(C49,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C49,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:J49" xr:uid="{F4D50087-81CA-4121-AC19-488D7706F9F6}"/>
   <conditionalFormatting sqref="G3:G48 H48:I48">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="21" priority="8">
       <formula>COUNTIF($Q$3:$AD$3,G3)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G48 H48:I48">
-    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49:I49">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="19" priority="6">
       <formula>COUNTIF($Q$3:$AD$3,G49)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G49:I49">
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J49">
+    <cfRule type="expression" dxfId="15" priority="23">
+      <formula>#REF!=1</formula>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4314,8 +4944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44142A8A-AFDD-49DF-95F7-861634CDED16}">
   <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7234,4 +7864,507 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId136"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279EA41E-7727-4698-8E10-FD63D59C9993}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27" thickBot="1">
+      <c r="A1" s="19" t="s">
+        <v>454</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>455</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A2" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>458</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A3" s="19" t="s">
+        <v>460</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>461</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27" thickBot="1">
+      <c r="A4" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>463</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A5" s="19" t="s">
+        <v>465</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A6" s="19" t="s">
+        <v>467</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>468</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27" thickBot="1">
+      <c r="A7" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>470</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="27" thickBot="1">
+      <c r="A8" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27" thickBot="1">
+      <c r="A9" s="19" t="s">
+        <v>471</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>472</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="27" thickBot="1">
+      <c r="A10" s="19" t="s">
+        <v>474</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>475</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A11" s="19" t="s">
+        <v>476</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>477</v>
+      </c>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="27" thickBot="1">
+      <c r="A12" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>479</v>
+      </c>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="39.75" thickBot="1">
+      <c r="A13" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>481</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="39.75" thickBot="1">
+      <c r="A14" s="19" t="s">
+        <v>482</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>483</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="27" thickBot="1">
+      <c r="A15" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="27" thickBot="1">
+      <c r="A16" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="27" thickBot="1">
+      <c r="A17" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>486</v>
+      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="27" thickBot="1">
+      <c r="A18" s="19" t="s">
+        <v>487</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>488</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="27" thickBot="1">
+      <c r="A19" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>489</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>490</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="27" thickBot="1">
+      <c r="A20" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>492</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>493</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="27" thickBot="1">
+      <c r="A21" s="19" t="s">
+        <v>494</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="27" thickBot="1">
+      <c r="A22" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>496</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="27" thickBot="1">
+      <c r="A23" s="19" t="s">
+        <v>497</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="27" thickBot="1">
+      <c r="A24" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>500</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="27" thickBot="1">
+      <c r="A25" s="19" t="s">
+        <v>462</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>501</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="39.75" thickBot="1">
+      <c r="A26" s="19" t="s">
+        <v>502</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>287</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>503</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A27" s="19" t="s">
+        <v>504</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="39.75" thickBot="1">
+      <c r="A28" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="39.75" thickBot="1">
+      <c r="A29" s="19" t="s">
+        <v>506</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="39.75" thickBot="1">
+      <c r="A30" s="19" t="s">
+        <v>508</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A31" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="27" thickBot="1">
+      <c r="A32" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="39.75" thickBot="1">
+      <c r="A33" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>424</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="27" thickBot="1">
+      <c r="A34" s="19" t="s">
+        <v>510</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A35" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A36" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="27" thickBot="1">
+      <c r="A37" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="27" thickBot="1">
+      <c r="A38" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="27" thickBot="1">
+      <c r="A39" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update ps ebanxs and logo pagseguro
</commit_message>
<xml_diff>
--- a/src/main/java/utility/logo.xlsx
+++ b/src/main/java/utility/logo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\project3ds\src\main\java\utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59861F5B-3B8F-4245-8929-FE3BD948DDE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E133BA-66FC-41D7-8A7C-3F1FC40540A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20385" yWindow="-10920" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8415" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="psname" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="1290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="1290">
   <si>
     <t>efectycolombia</t>
   </si>
@@ -4349,7 +4349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4518,6 +4518,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4527,22 +4533,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4682,6 +4678,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFABAB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5016,11 +5019,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7632,20 +7635,20 @@
         <v>383</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="87" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="87">
-        <v>1</v>
+    <row r="66" spans="1:11" s="85" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0</v>
       </c>
       <c r="B66" s="17">
         <v>180</v>
       </c>
-      <c r="C66" s="87" t="s">
+      <c r="C66" s="85" t="s">
         <v>371</v>
       </c>
-      <c r="D66" s="87" t="s">
+      <c r="D66" s="85" t="s">
         <v>370</v>
       </c>
-      <c r="E66" s="87" t="s">
+      <c r="E66" s="85" t="s">
         <v>1288</v>
       </c>
       <c r="F66" s="32" t="s">
@@ -7661,27 +7664,27 @@
       <c r="I66" s="32">
         <v>86844</v>
       </c>
-      <c r="J66" s="87">
+      <c r="J66" s="85">
         <v>94</v>
       </c>
       <c r="K66" s="32" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="87" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="87">
-        <v>1</v>
+    <row r="67" spans="1:11" s="85" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0</v>
       </c>
       <c r="B67" s="17">
         <v>203</v>
       </c>
-      <c r="C67" s="87" t="s">
+      <c r="C67" s="85" t="s">
         <v>203</v>
       </c>
-      <c r="D67" s="87" t="s">
+      <c r="D67" s="85" t="s">
         <v>372</v>
       </c>
-      <c r="E67" s="87" t="s">
+      <c r="E67" s="85" t="s">
         <v>1289</v>
       </c>
       <c r="F67" s="32" t="s">
@@ -7697,47 +7700,88 @@
       <c r="I67" s="32">
         <v>86844</v>
       </c>
-      <c r="J67" s="87">
+      <c r="J67" s="85">
         <v>94</v>
       </c>
       <c r="K67" s="32" t="s">
         <v>427</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="85" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="85">
+        <v>1</v>
+      </c>
+      <c r="B68" s="17">
+        <v>93</v>
+      </c>
+      <c r="C68" s="85" t="s">
+        <v>175</v>
+      </c>
+      <c r="D68" s="85" t="s">
+        <v>323</v>
+      </c>
+      <c r="E68" s="85" t="s">
+        <v>175</v>
+      </c>
+      <c r="F68" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="G68" s="84" t="str">
+        <f>IF(ISNA(VLOOKUP(C68,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C68,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
+      <c r="H68" s="32">
+        <v>99894</v>
+      </c>
+      <c r="I68" s="32">
+        <v>86844</v>
+      </c>
+      <c r="J68" s="85">
+        <v>30</v>
+      </c>
+      <c r="K68" s="32" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:L51" xr:uid="{F4D50087-81CA-4121-AC19-488D7706F9F6}"/>
   <conditionalFormatting sqref="K50:L50 K52:K53">
-    <cfRule type="expression" dxfId="23" priority="14">
+    <cfRule type="expression" dxfId="23" priority="15">
       <formula>COUNTIF($S$3:$AF$3,K50)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50:L50">
-    <cfRule type="duplicateValues" dxfId="22" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51:L51">
-    <cfRule type="expression" dxfId="21" priority="12">
+    <cfRule type="expression" dxfId="21" priority="13">
       <formula>COUNTIF($S$3:$AF$3,K51)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51:L51 K52:K53">
-    <cfRule type="duplicateValues" dxfId="20" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G41 G45:G66">
-    <cfRule type="expression" dxfId="19" priority="29">
+    <cfRule type="expression" dxfId="19" priority="30">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="expression" dxfId="18" priority="6">
+    <cfRule type="expression" dxfId="18" priority="7">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44">
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G67">
+    <cfRule type="expression" dxfId="16" priority="2">
+      <formula>#REF!=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G68">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!=1</formula>
     </cfRule>
@@ -18364,59 +18408,59 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:C74">
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="15" priority="14">
       <formula>COUNTIF($Q$3:$AD$3,B2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75:C75">
-    <cfRule type="expression" dxfId="15" priority="11">
+    <cfRule type="expression" dxfId="14" priority="11">
       <formula>COUNTIF($Q$3:$AD$3,B75)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75">
-    <cfRule type="duplicateValues" dxfId="14" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76:C76">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>COUNTIF($Q$3:$AD$3,B76)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76">
-    <cfRule type="duplicateValues" dxfId="11" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77:C82">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>COUNTIF($Q$3:$AD$3,B77)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77:C82">
-    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77:B82">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83:C83">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>COUNTIF($Q$3:$AD$3,B83)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C74">
-    <cfRule type="duplicateValues" dxfId="3" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B74">
-    <cfRule type="duplicateValues" dxfId="2" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="21"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26783,7 +26827,7 @@
       <c r="F2" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="G2" s="84"/>
+      <c r="G2" s="86"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -26818,7 +26862,7 @@
       <c r="F3" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="G3" s="85"/>
+      <c r="G3" s="87"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -26853,7 +26897,7 @@
       <c r="F4" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="G4" s="85"/>
+      <c r="G4" s="87"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -26888,7 +26932,7 @@
       <c r="F5" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="G5" s="85"/>
+      <c r="G5" s="87"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -26923,7 +26967,7 @@
       <c r="F6" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G6" s="85"/>
+      <c r="G6" s="87"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -26958,7 +27002,7 @@
       <c r="F7" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="G7" s="85"/>
+      <c r="G7" s="87"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -26993,7 +27037,7 @@
       <c r="F8" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="G8" s="85"/>
+      <c r="G8" s="87"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -27028,7 +27072,7 @@
       <c r="F9" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="G9" s="85"/>
+      <c r="G9" s="87"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -27063,7 +27107,7 @@
       <c r="F10" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="G10" s="85"/>
+      <c r="G10" s="87"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -27098,7 +27142,7 @@
       <c r="F11" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="G11" s="86"/>
+      <c r="G11" s="88"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>

</xml_diff>

<commit_message>
update ps test for UI changing
</commit_message>
<xml_diff>
--- a/src/main/java/utility/logo.xlsx
+++ b/src/main/java/utility/logo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\project3ds\src\main\java\utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0486535D-D762-41A4-BA53-7D431EFD5D9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823140E3-0CEE-41FB-8FCD-DE11BABDA980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8415" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20385" yWindow="-10920" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="psname" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="1299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="1300">
   <si>
     <t>efectycolombia</t>
   </si>
@@ -3961,6 +3961,9 @@
   </si>
   <si>
     <t>rupay</t>
+  </si>
+  <si>
+    <t>openbucks_usca</t>
   </si>
 </sst>
 </file>
@@ -4376,7 +4379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4550,6 +4553,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4987,11 +4993,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6644,7 +6650,7 @@
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B41">
         <f>VLOOKUP(C41,shortcode!$C$1:$D$200,2,FALSE)</f>
@@ -6685,7 +6691,7 @@
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B42">
         <f>VLOOKUP(C42,shortcode!$C$1:$D$200,2,FALSE)</f>
@@ -6725,7 +6731,7 @@
     </row>
     <row r="43" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B43">
         <f>VLOOKUP(C43,shortcode!$C$1:$D$200,2,FALSE)</f>
@@ -6765,7 +6771,7 @@
     </row>
     <row r="44" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B44">
         <f>VLOOKUP(C44,shortcode!$C$1:$D$200,2,FALSE)</f>
@@ -6805,7 +6811,7 @@
     </row>
     <row r="45" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B45">
         <f>VLOOKUP(C45,shortcode!$C$1:$D$200,2,FALSE)</f>
@@ -6845,7 +6851,7 @@
     </row>
     <row r="46" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B46">
         <f>VLOOKUP(C46,shortcode!$C$1:$D$200,2,FALSE)</f>
@@ -6885,7 +6891,7 @@
     </row>
     <row r="47" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B47">
         <f>VLOOKUP(C47,shortcode!$C$1:$D$200,2,FALSE)</f>
@@ -6925,7 +6931,7 @@
     </row>
     <row r="48" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B48">
         <f>VLOOKUP(C48,shortcode!$C$1:$D$200,2,FALSE)</f>
@@ -7836,7 +7842,7 @@
       </c>
     </row>
     <row r="72" spans="1:11" s="85" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="85">
+      <c r="A72">
         <v>0</v>
       </c>
       <c r="B72" s="17">
@@ -7871,7 +7877,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>0</v>
       </c>
@@ -7890,6 +7896,10 @@
       <c r="F73" s="32" t="s">
         <v>1287</v>
       </c>
+      <c r="G73" s="87" t="str">
+        <f>IF(ISNA(VLOOKUP(C73,logoName!$B$2:$D$39,3,FALSE)),"",VLOOKUP(C73,logoName!$B$2:$D$39,3,FALSE))</f>
+        <v/>
+      </c>
       <c r="H73" s="32">
         <v>99894</v>
       </c>
@@ -7901,6 +7911,41 @@
       </c>
       <c r="K73" s="32" t="s">
         <v>816</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74" s="17">
+        <v>170</v>
+      </c>
+      <c r="C74" s="85" t="s">
+        <v>320</v>
+      </c>
+      <c r="D74" s="85" t="s">
+        <v>319</v>
+      </c>
+      <c r="E74" s="85" t="s">
+        <v>320</v>
+      </c>
+      <c r="F74" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="G74" s="87" t="s">
+        <v>1299</v>
+      </c>
+      <c r="H74" s="32">
+        <v>99894</v>
+      </c>
+      <c r="I74" s="32">
+        <v>86844</v>
+      </c>
+      <c r="J74" s="85">
+        <v>2</v>
+      </c>
+      <c r="K74" s="32" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -26394,8 +26439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279EA41E-7727-4698-8E10-FD63D59C9993}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26951,7 +26996,7 @@
       <c r="F2" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="G2" s="87"/>
+      <c r="G2" s="88"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -26986,7 +27031,7 @@
       <c r="F3" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="G3" s="88"/>
+      <c r="G3" s="89"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -27021,7 +27066,7 @@
       <c r="F4" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="G4" s="88"/>
+      <c r="G4" s="89"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -27056,7 +27101,7 @@
       <c r="F5" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="G5" s="88"/>
+      <c r="G5" s="89"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -27091,7 +27136,7 @@
       <c r="F6" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G6" s="88"/>
+      <c r="G6" s="89"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -27126,7 +27171,7 @@
       <c r="F7" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="G7" s="88"/>
+      <c r="G7" s="89"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -27161,7 +27206,7 @@
       <c r="F8" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="G8" s="88"/>
+      <c r="G8" s="89"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -27196,7 +27241,7 @@
       <c r="F9" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="G9" s="88"/>
+      <c r="G9" s="89"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -27231,7 +27276,7 @@
       <c r="F10" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="G10" s="88"/>
+      <c r="G10" s="89"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -27266,7 +27311,7 @@
       <c r="F11" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="G11" s="89"/>
+      <c r="G11" s="90"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>

</xml_diff>